<commit_message>
import export indicator added but need to bug
</commit_message>
<xml_diff>
--- a/static/SampleExcel/IndicatorSample.xlsx
+++ b/static/SampleExcel/IndicatorSample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/MoPD/Time-Series-Data/static/SampleExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AC3755-4473-8E41-A3EE-AC84E5058CAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB9A959-BC65-184E-BB71-9B6BBE51BC34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>title_ENG</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>parent</t>
-  </si>
-  <si>
-    <t>for_category</t>
   </si>
   <si>
     <t>measurement</t>
@@ -391,11 +388,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -405,7 +402,7 @@
     <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -421,9 +418,6 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>